<commit_message>
Nov 12 2018 Morning
</commit_message>
<xml_diff>
--- a/AppliedAI/Models_Finalize.xlsx
+++ b/AppliedAI/Models_Finalize.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="909" firstSheet="7" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="909" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="162">
   <si>
     <t>Missing Values</t>
   </si>
@@ -889,12 +889,38 @@
     <t>max_iter : int, default: 300
 Maximum number of iterations of the k-means algorithm for a single run.</t>
   </si>
+  <si>
+    <t>2. What are the basic assumptions to be made for linear regression?(https://www.appliedaicourse.com/course/applied-ai-course-online/lessons/geometric-intuition-1-2-copy-8/)</t>
+  </si>
+  <si>
+    <t>3. What is the difference between stochastic gradient descent (SGD) and gradient descent (GD)?(https://stats.stackexchange.com/questions/317675/gradient-descent-gd-vs-stochastic-gradient-descent-sgd)</t>
+  </si>
+  <si>
+    <t>4. When would you use GD over SDG, and vice-versa?(https://elitedatascience.com/machine-learning-interview-questions-answers)</t>
+  </si>
+  <si>
+    <t>5. How do you decide whether your linear regression model fits the data?(https://www.researchgate.net/post/What_statistical_test_is_required_to_assess_goodness_of_fit_of_a_linear_or_nonlinear_regression_equation)</t>
+  </si>
+  <si>
+    <t>6. Is it possible to perform logistic regression with Microsoft Excel?(https://www.youtube.com/watch?v=EKRjDurXau0)</t>
+  </si>
+  <si>
+    <t>7. When will you use classification over regression?(https://www.quora.com/When-will-you-use-classification-over-regression)</t>
+  </si>
+  <si>
+    <t>8. Why isn’t Logistic Regression called Logistic Classification?(Refer :https://stats.stackexchange.com/questions/127042/why-isnt-logistic-regression-called-logistic-classification/127044)</t>
+  </si>
+  <si>
+    <t>1. After analysing the model, your manager has informed that your regression model is suffering from multicollinearity. How would you check if he’s true? Without losing any information, can you still build a better model?(https://google-interview-hacks.blogspot.in/2017/04/after-analyzing-model-your-manager-has.html)
+To check multicollinearity, we can create a correlation matrix to identify &amp; remove variables having correlation above 75% (deciding a threshold is subjective). In addition, we can use calculate VIF (variance inflation factor) to check the presence of multicollinearity. VIF value &lt;= 4 suggests no multicollinearity whereas a value of &gt;= 10 implies serious multicollinearity. Also, we can use tolerance as an indicator of multicollinearity.
+But, removing correlated variables might lead to loss of information. In order to retain those variables, we can use penalized regression models like ridge or lasso regression. Also, we can add some random noise in correlated variable so that the variables become different from each other. But, adding noise might affect the prediction accuracy, hence this approach should be carefully used.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -991,6 +1017,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1055,7 +1086,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1146,6 +1177,10 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1158,9 +1193,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1469,7 +1503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1483,77 +1517,77 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="23.25"/>
   <cols>
     <col min="1" max="1" width="32" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="16" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" s="23" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" s="23" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" s="23" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1">
       <c r="A10" s="16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1">
       <c r="A11" s="16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1">
       <c r="A12" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1">
       <c r="A13" s="16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1">
       <c r="A14" s="16" t="s">
         <v>110</v>
       </c>
@@ -1579,14 +1613,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -1594,7 +1628,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -1602,7 +1636,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1644,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="22" t="s">
         <v>43</v>
       </c>
@@ -1618,7 +1652,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
@@ -1626,13 +1660,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="22" t="s">
         <v>3</v>
       </c>
@@ -1640,21 +1674,21 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="75">
+      <c r="A9" s="36"/>
       <c r="B9" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="22" t="s">
         <v>8</v>
       </c>
@@ -1662,7 +1696,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="22" t="s">
         <v>47</v>
       </c>
@@ -1670,7 +1704,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
@@ -1678,7 +1712,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="22" t="s">
         <v>73</v>
       </c>
@@ -1686,7 +1720,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="22" t="s">
         <v>12</v>
       </c>
@@ -1694,13 +1728,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="22" t="s">
         <v>14</v>
       </c>
@@ -1708,7 +1742,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
@@ -1716,7 +1750,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
         <v>15</v>
       </c>
@@ -1724,7 +1758,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
         <v>16</v>
       </c>
@@ -1732,7 +1766,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="22" t="s">
         <v>27</v>
       </c>
@@ -1740,7 +1774,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="22" t="s">
         <v>35</v>
       </c>
@@ -1748,7 +1782,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
         <v>24</v>
       </c>
@@ -1756,45 +1790,45 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:2" ht="15">
+      <c r="A23" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+    <row r="24" spans="1:2" ht="45">
+      <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+    <row r="25" spans="1:2" ht="15">
+      <c r="A25" s="36"/>
       <c r="B25" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:2" ht="15">
+      <c r="A26" s="36"/>
       <c r="B26" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:2" ht="75">
+      <c r="A27" s="36"/>
       <c r="B27" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:2" ht="15">
+      <c r="A28" s="36"/>
       <c r="B28" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="22" t="s">
         <v>29</v>
       </c>
@@ -1802,7 +1836,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="37.5">
       <c r="A30" s="12" t="s">
         <v>31</v>
       </c>
@@ -1810,8 +1844,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" ht="15"/>
+    <row r="34" s="1" customFormat="1" ht="15"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A8:A9"/>
@@ -1836,14 +1870,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -1851,7 +1885,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -1859,7 +1893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="31" t="s">
         <v>43</v>
       </c>
@@ -1875,7 +1909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="31" t="s">
         <v>1</v>
       </c>
@@ -1883,13 +1917,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="31" t="s">
         <v>3</v>
       </c>
@@ -1897,19 +1931,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="39"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
@@ -1917,13 +1951,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="31" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="31" t="s">
         <v>10</v>
       </c>
@@ -1931,7 +1965,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="31" t="s">
         <v>73</v>
       </c>
@@ -1939,7 +1973,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="31" t="s">
         <v>12</v>
       </c>
@@ -1947,13 +1981,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="28" t="s">
         <v>14</v>
       </c>
@@ -1961,7 +1995,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="28" t="s">
         <v>25</v>
       </c>
@@ -1969,13 +2003,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="28" t="s">
         <v>16</v>
       </c>
@@ -1983,7 +2017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="57.75">
       <c r="A20" s="28" t="s">
         <v>27</v>
       </c>
@@ -1991,7 +2025,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="28" t="s">
         <v>35</v>
       </c>
@@ -1999,7 +2033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="28" t="s">
         <v>24</v>
       </c>
@@ -2007,50 +2041,50 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:2" ht="30">
+      <c r="A23" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+    <row r="24" spans="1:2" ht="30">
+      <c r="A24" s="36"/>
       <c r="B24" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+    <row r="25" spans="1:2" ht="15">
+      <c r="A25" s="36"/>
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:2" ht="15">
+      <c r="A26" s="36"/>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="36"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:2" ht="15">
+      <c r="A28" s="36"/>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="28" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="37.5">
       <c r="A30" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="7"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" ht="15"/>
+    <row r="34" s="1" customFormat="1" ht="15"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A8:A9"/>
@@ -2071,7 +2105,7 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2085,7 +2119,7 @@
       <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2099,7 +2133,7 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2116,14 +2150,14 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -2131,7 +2165,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -2139,7 +2173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +2181,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="32" t="s">
         <v>43</v>
       </c>
@@ -2155,7 +2189,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
@@ -2163,7 +2197,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="29" t="s">
         <v>2</v>
       </c>
@@ -2171,7 +2205,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="32" t="s">
         <v>3</v>
       </c>
@@ -2179,37 +2213,37 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:2" ht="30">
+      <c r="A8" s="39" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="39"/>
       <c r="B9" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="39"/>
       <c r="B10" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="39" t="s">
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="39"/>
+      <c r="B11" s="35" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
+    <row r="12" spans="1:2" ht="15">
+      <c r="A12" s="39"/>
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="32" t="s">
         <v>135</v>
       </c>
@@ -2217,7 +2251,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="32" t="s">
         <v>8</v>
       </c>
@@ -2225,7 +2259,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="32" t="s">
         <v>47</v>
       </c>
@@ -2233,7 +2267,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="30">
       <c r="A16" s="32" t="s">
         <v>10</v>
       </c>
@@ -2241,37 +2275,37 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="32" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="32" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="29" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="30" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" s="30" t="s">
         <v>15</v>
       </c>
@@ -2279,13 +2313,13 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="30" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="29.25">
       <c r="A24" s="30" t="s">
         <v>27</v>
       </c>
@@ -2293,72 +2327,71 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="36" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:2" ht="30">
+      <c r="A28" s="36"/>
       <c r="B28" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:2" ht="75">
+      <c r="A29" s="36"/>
       <c r="B29" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:2" ht="45">
+      <c r="A30" s="36"/>
       <c r="B30" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+    <row r="31" spans="1:2" ht="30">
+      <c r="A31" s="36"/>
       <c r="B31" s="7" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:2" ht="15">
+      <c r="A32" s="36"/>
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="30" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="37.5">
       <c r="A34" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
     </row>
@@ -2383,7 +2416,7 @@
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2397,7 +2430,7 @@
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2411,7 +2444,7 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2421,21 +2454,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="34" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -2446,7 +2479,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>140</v>
       </c>
@@ -2461,20 +2494,20 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -2482,7 +2515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -2490,7 +2523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -2498,7 +2531,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -2506,7 +2539,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -2514,7 +2547,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
@@ -2522,7 +2555,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -2530,27 +2563,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
@@ -2558,7 +2591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="10" t="s">
         <v>47</v>
       </c>
@@ -2566,7 +2599,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="45">
       <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
@@ -2574,7 +2607,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="10" t="s">
         <v>73</v>
       </c>
@@ -2582,7 +2615,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2590,13 +2623,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
@@ -2604,7 +2637,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
@@ -2612,7 +2645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="30">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
@@ -2620,7 +2653,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
@@ -2628,7 +2661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="45">
       <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
@@ -2636,7 +2669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
@@ -2644,7 +2677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="10" t="s">
         <v>24</v>
       </c>
@@ -2652,7 +2685,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="60">
       <c r="A24" s="10" t="s">
         <v>20</v>
       </c>
@@ -2660,27 +2693,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:2" ht="45">
+      <c r="A25" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:2" ht="135">
+      <c r="A26" s="36"/>
       <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:2" ht="30">
+      <c r="A27" s="36"/>
       <c r="B27" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="30">
       <c r="A28" s="10" t="s">
         <v>29</v>
       </c>
@@ -2688,12 +2721,52 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="60">
       <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="142.5">
+      <c r="B30" s="40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="28.5">
+      <c r="B31" s="40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="28.5">
+      <c r="B32" s="40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" ht="42.75">
+      <c r="B34" s="40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="28.5">
+      <c r="B37" s="40" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2720,14 +2793,14 @@
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="33.42578125" style="13" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -2735,7 +2808,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -2743,7 +2816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -2751,13 +2824,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -2765,7 +2838,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -2773,7 +2846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -2781,63 +2854,63 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="36" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="36"/>
       <c r="B9" s="20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="36"/>
       <c r="B10" s="20" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="36"/>
       <c r="B11" s="21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+    <row r="12" spans="1:2" ht="90">
+      <c r="A12" s="36"/>
       <c r="B12" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+    <row r="13" spans="1:2" ht="90">
+      <c r="A13" s="36"/>
       <c r="B13" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+    <row r="14" spans="1:2" ht="30">
+      <c r="A14" s="36"/>
       <c r="B14" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+    <row r="15" spans="1:2" ht="60">
+      <c r="A15" s="36"/>
       <c r="B15" s="21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+    <row r="16" spans="1:2" ht="15">
+      <c r="A16" s="36"/>
       <c r="B16" s="21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -2845,7 +2918,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -2853,7 +2926,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="11" t="s">
         <v>80</v>
       </c>
@@ -2861,13 +2934,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="11" t="s">
         <v>12</v>
       </c>
@@ -2875,7 +2948,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" s="11" t="s">
         <v>13</v>
       </c>
@@ -2883,7 +2956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="11" t="s">
         <v>14</v>
       </c>
@@ -2891,19 +2964,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="11" t="s">
         <v>16</v>
       </c>
@@ -2911,7 +2984,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="90">
       <c r="A27" s="11" t="s">
         <v>27</v>
       </c>
@@ -2919,7 +2992,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="30">
       <c r="A28" s="11" t="s">
         <v>35</v>
       </c>
@@ -2927,63 +3000,63 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+    <row r="31" spans="1:2" ht="30">
+      <c r="A31" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:2" ht="30">
+      <c r="A32" s="36"/>
       <c r="B32" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+    <row r="33" spans="1:2" ht="45">
+      <c r="A33" s="36"/>
       <c r="B33" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+    <row r="34" spans="1:2" ht="30">
+      <c r="A34" s="36"/>
       <c r="B34" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
+    <row r="35" spans="1:2" ht="90">
+      <c r="A35" s="36"/>
       <c r="B35" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+    <row r="36" spans="1:2" ht="15">
+      <c r="A36" s="36"/>
       <c r="B36" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="34"/>
+    <row r="37" spans="1:2" ht="15">
+      <c r="A37" s="36"/>
       <c r="B37" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="30">
       <c r="A38" s="11" t="s">
         <v>29</v>
       </c>
@@ -2991,13 +3064,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="37.5">
       <c r="A39" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="7"/>
     </row>
-    <row r="40" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="45">
       <c r="A40" s="12" t="s">
         <v>64</v>
       </c>
@@ -3005,7 +3078,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="45">
       <c r="A41" s="11" t="s">
         <v>59</v>
       </c>
@@ -3013,10 +3086,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="B43" s="1"/>
     </row>
   </sheetData>
@@ -3040,14 +3113,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="33.42578125" style="13" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -3055,7 +3128,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -3063,83 +3136,83 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="36"/>
       <c r="B10" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="36"/>
       <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+    <row r="12" spans="1:2" ht="15">
+      <c r="A12" s="36"/>
       <c r="B12" s="19"/>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+    <row r="13" spans="1:2" ht="15">
+      <c r="A13" s="36"/>
       <c r="B13" s="19"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="10" t="s">
         <v>10</v>
       </c>
@@ -3147,49 +3220,49 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="4"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="10" t="s">
         <v>27</v>
       </c>
@@ -3197,7 +3270,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="30">
       <c r="A25" s="10" t="s">
         <v>35</v>
       </c>
@@ -3205,41 +3278,41 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+    <row r="28" spans="1:2" ht="60">
+      <c r="A28" s="36" t="s">
         <v>92</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:2" ht="15">
+      <c r="A29" s="36"/>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:2" ht="15">
+      <c r="A30" s="36"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="10" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="37.5">
       <c r="A32" s="12" t="s">
         <v>31</v>
       </c>
@@ -3265,14 +3338,14 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="33.42578125" style="13" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -3280,7 +3353,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -3288,7 +3361,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -3296,13 +3369,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="11" t="s">
         <v>1</v>
       </c>
@@ -3310,7 +3383,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -3318,7 +3391,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="11" t="s">
         <v>3</v>
       </c>
@@ -3326,29 +3399,29 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="45">
+      <c r="A8" s="36" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="36"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="36"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
@@ -3356,7 +3429,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
@@ -3364,7 +3437,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="11" t="s">
         <v>80</v>
       </c>
@@ -3372,13 +3445,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="11" t="s">
         <v>12</v>
       </c>
@@ -3386,7 +3459,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="11" t="s">
         <v>13</v>
       </c>
@@ -3394,7 +3467,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
@@ -3402,19 +3475,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="11" t="s">
         <v>16</v>
       </c>
@@ -3422,7 +3495,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="45">
       <c r="A22" s="11" t="s">
         <v>27</v>
       </c>
@@ -3430,90 +3503,90 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:2" ht="15">
+      <c r="A26" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="36"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
+    <row r="28" spans="1:2" ht="15">
+      <c r="A28" s="36"/>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
+    <row r="29" spans="1:2" ht="15">
+      <c r="A29" s="36"/>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
+    <row r="30" spans="1:2" ht="15">
+      <c r="A30" s="36"/>
       <c r="B30" s="7"/>
     </row>
-    <row r="31" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+    <row r="31" spans="1:2" ht="15">
+      <c r="A31" s="36"/>
       <c r="B31" s="7"/>
     </row>
-    <row r="32" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
+    <row r="32" spans="1:2" ht="15">
+      <c r="A32" s="36"/>
       <c r="B32" s="7"/>
     </row>
-    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
+    <row r="33" spans="1:2" ht="15">
+      <c r="A33" s="36"/>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
+    <row r="34" spans="1:2" ht="15">
+      <c r="A34" s="36"/>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="7"/>
     </row>
-    <row r="36" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="37.5">
       <c r="A36" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B36" s="7"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="12" t="s">
         <v>64</v>
       </c>
       <c r="B37" s="7"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="B40" s="1"/>
     </row>
   </sheetData>
@@ -3536,7 +3609,7 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3550,7 +3623,7 @@
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3564,14 +3637,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="144.5703125" style="8" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="23.25">
       <c r="A1" s="9" t="s">
         <v>38</v>
       </c>
@@ -3579,7 +3652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
@@ -3587,170 +3660,170 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="17" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="36"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="36"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="5"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="17" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="6"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="17" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="17" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+    <row r="25" spans="1:2" ht="15">
+      <c r="A25" s="36" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="7"/>
     </row>
-    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+    <row r="26" spans="1:2" ht="15">
+      <c r="A26" s="36"/>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="36"/>
       <c r="B27" s="7"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="17" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="7"/>
     </row>
-    <row r="29" spans="1:2" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="37.5">
       <c r="A29" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B29" s="7"/>
     </row>
-    <row r="30" spans="1:2" ht="360" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+    <row r="30" spans="1:2" ht="360">
+      <c r="A30" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A31" s="36"/>
+    <row r="31" spans="1:2" ht="195">
+      <c r="A31" s="38"/>
       <c r="B31" s="27" t="s">
         <v>114</v>
       </c>
@@ -3777,9 +3850,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>115</v>
       </c>

</xml_diff>